<commit_message>
Add Notebook And Data Preprocessing
</commit_message>
<xml_diff>
--- a/CARBRAIN/data/output/xlsx/auto.xlsx
+++ b/CARBRAIN/data/output/xlsx/auto.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3589,6 +3589,942 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Dacia</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sandero</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>€ 1 000,-5</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Pas d'information</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>100 326 km</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>10/2012</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>55 kW (75 CH)</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">55 kW (75 CH) Boîte manuelle 1 149 cm³ 5 4 1 050 kg </t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/dacia-sandero-1-2i-75pk-schadewagen-airco-blueto-essence-gris-5a4524ae-2307-499f-bc27-9601fba15f4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Peugeot</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>€ 5 990,-5</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>118 000 km</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>01/2016</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>55 kW (75 CH)</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">55 kW (75 CH) Boîte manuelle 1 560 cm³ 5 4 1 140 kg </t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/peugeot-208-1-6-bluehdi-style-diesel-blanc-bd52d51c-57b3-4c08-b2ee-b0dcc25c5be4</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Volkswagen</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Polo</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>€ 6 990,-5</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>75 000 km</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>03/2013</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>51 kW (69 CH)</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">51 kW (69 CH) Boîte manuelle 1 198 cm³ 5 3 1 067 kg </t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/volkswagen-polo-1-2-essence-70cv-climatisation-essence-blanc-7419a210-815e-4abd-8263-5c1cbe07091e</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Insignia</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>€ 7 250,-5</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>128 548 km</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>03/2016</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>100 kW (136 CH)</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">100 kW (136 CH) Boîte manuelle 1 598 cm³ 6 4 1 613 kg </t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/opel-insignia-sports-tourer-1-6-cdti-ecoflex-cosmo-diesel-blanc-f8b601d1-1bcf-4bb8-b08d-3ce6351d1858</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Peugeot</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Partner</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>€ 1 950,-5</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Pas d'information</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>131 000 km</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>06/2004</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>80 kW (109 CH)</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">80 kW (109 CH) Boîte manuelle 1 587 cm³ 5 4 1 260 kg </t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/peugeot-partner-1-6i-benzine-bj-2004-131000km-5-zitplaatsen-airco-essence-rouge-66044004-8b6f-4b72-aace-b74bfb15e962</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Citroen</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>€ 10 250,-5</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>19 599 km</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>10/2022</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>61 kW (83 CH)</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">61 kW (83 CH) Boîte manuelle 1 199 cm³ 5 3 980 kg </t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/citroen-c3-1-2i-puretech-you-s-essence-rouge-7a6c2a29-4e6f-4016-b6e6-162b32206bc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Mercedes-Benz</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>B 180</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>€ 2 750,-5</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Prix correct</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>189 000 km</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Boîte automatique</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>06/2005</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>80 kW (109 CH)</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">80 kW (109 CH) Boîte automatique 1 991 cm³ 1 4 1 470 kg </t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/mercedes-benz-b-180-cdi-automatique-bj-2005-189000km-diesel-brun-08a6a9c1-263f-430e-87d3-e525b30c7785</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Opel</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Insignia</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>€ 3 600,-5</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>200 240 km</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>03/2013</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>96 kW (131 CH)</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">96 kW (131 CH) Boîte manuelle 1 956 cm³ 6 4 1 610 kg </t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/opel-insignia-sports-tourer-2-0-cdti-cosmo-dpf-diesel-gris-6ad70203-4e1e-4928-94a4-2039f729ad3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Peugeot</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>€ 4 950,-5</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>118 431 km</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>04/2018</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>50 kW (68 CH)</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50 kW (68 CH) Boîte manuelle 1 199 cm³ 5 3 1 035 kg </t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/peugeot-208-1-2i-puretech-access-essence-rouge-ee538c2c-2a94-4294-8e16-015a1e66a544</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Skoda</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Rapid/Spaceback</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>€ 7 450,-5</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>100 063 km</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>08/2015</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>77 kW (105 CH)</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">77 kW (105 CH) Boîte manuelle 1 598 cm³ 5 4 1 265 kg </t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/skoda-rapid-spaceback-rapid-1-6-cr-tdi-elegance-diesel-noir-b81f55d8-98c2-46c7-98d7-e1bd9d29068e</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Mazda</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>€ 2 950,-5</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>149 218 km</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>06/2007</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>55 kW (75 CH)</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">55 kW (75 CH) Boîte manuelle 1 242 cm³ 5 4 1 125 kg </t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/mazda-2-1-25-essence-75cv-essence-argent-392f5a5e-0038-4f56-bdb8-b48b96e58351</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BMW</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>216</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>€ 9 950,-5</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>138 000 km</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>01/2018</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>75 kW (102 CH)</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">75 kW (102 CH) Boîte manuelle 1 499 cm³ 6 3 1 440 kg </t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/bmw-216-i-active-tourer-euro-6b-gps-navi-bluetooth-essence-gris-24ae4f29-68b4-4b32-97a1-7ce14aba3332</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Peugeot</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>308</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>€ 5 990,-5</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Très bon prix</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>118 000 km</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Boîte manuelle</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>01/2011</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Essence</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>88 kW (120 CH)</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Professionnel</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">88 kW (120 CH) Boîte manuelle 1 598 cm³ 5 4 1 555 kg </t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>https://www.autoscout24.be/fr/offres/peugeot-308-cc-1-6i-sport-pack-airco-garantie-prete-immatricul-essence-e57bcf32-9adc-4b18-a130-92b738dc1a62</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>